<commit_message>
adding more writing and fixing up results
</commit_message>
<xml_diff>
--- a/results/Office.Texture.blindSpotRotation.xlsx
+++ b/results/Office.Texture.blindSpotRotation.xlsx
@@ -128,8 +128,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,11 +607,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="202167536"/>
-        <c:axId val="202161656"/>
+        <c:axId val="199296240"/>
+        <c:axId val="199294672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="202167536"/>
+        <c:axId val="199296240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -633,7 +633,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
@@ -649,7 +648,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202161656"/>
+        <c:crossAx val="199294672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -657,7 +656,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202161656"/>
+        <c:axId val="199294672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -686,7 +685,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -703,14 +701,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202167536"/>
+        <c:crossAx val="199296240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -1604,11 +1601,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="202160872"/>
-        <c:axId val="202164008"/>
+        <c:axId val="199292320"/>
+        <c:axId val="199295064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="202160872"/>
+        <c:axId val="199292320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1617,7 +1614,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="202164008"/>
+        <c:crossAx val="199295064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1625,7 +1622,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202164008"/>
+        <c:axId val="199295064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -1638,14 +1635,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="202160872"/>
+        <c:crossAx val="199292320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2115,11 +2111,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="202166752"/>
-        <c:axId val="202168320"/>
+        <c:axId val="199295848"/>
+        <c:axId val="199288792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="202166752"/>
+        <c:axId val="199295848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2157,7 +2153,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202168320"/>
+        <c:crossAx val="199288792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2165,7 +2161,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202168320"/>
+        <c:axId val="199288792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2211,7 +2207,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202166752"/>
+        <c:crossAx val="199295848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2648,7 +2644,7 @@
   <dimension ref="A1:S52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+      <selection activeCell="Q48" sqref="Q48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,10 +2653,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -3552,7 +3548,7 @@
         <v>0</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="3"/>
+        <f>IF($L31=J31,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -3618,13 +3614,13 @@
         <v>0</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="Q32:Q50" si="8">IF($L32=J32,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" ref="A33:A50" si="8">A32+1</f>
+        <f t="shared" ref="A33:A50" si="9">A32+1</f>
         <v>3</v>
       </c>
       <c r="B33">
@@ -3684,13 +3680,13 @@
         <v>0</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B34">
@@ -3750,13 +3746,13 @@
         <v>0</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="B35">
@@ -3816,13 +3812,13 @@
         <v>0</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B36">
@@ -3882,13 +3878,13 @@
         <v>0</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="B37">
@@ -3948,13 +3944,13 @@
         <v>0</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="B38">
@@ -3962,31 +3958,31 @@
         <v>1.44723</v>
       </c>
       <c r="C38">
-        <f t="shared" ref="C38:I40" si="9">C14/$B38</f>
+        <f t="shared" ref="C38:I40" si="10">C14/$B38</f>
         <v>1.1606309985282228</v>
       </c>
       <c r="D38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.1355416899870785</v>
       </c>
       <c r="E38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.93754966384057814</v>
       </c>
       <c r="F38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.93938765780145517</v>
       </c>
       <c r="G38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.1381743053972069</v>
       </c>
       <c r="H38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.4642178506526262</v>
       </c>
       <c r="I38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.93989897942966905</v>
       </c>
       <c r="J38">
@@ -4014,13 +4010,13 @@
         <v>0</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="B39">
@@ -4028,31 +4024,31 @@
         <v>7.1884899999999998</v>
       </c>
       <c r="C39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.23763683332660965</v>
       </c>
       <c r="D39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.94435270828783235</v>
       </c>
       <c r="E39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.20096710157487874</v>
       </c>
       <c r="F39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.0042748894413152</v>
       </c>
       <c r="G39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.22316786974733221</v>
       </c>
       <c r="H39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2013496575775997</v>
       </c>
       <c r="I39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.24897301102178623</v>
       </c>
       <c r="J39">
@@ -4080,13 +4076,13 @@
         <v>0</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="B40">
@@ -4094,31 +4090,31 @@
         <v>9.9110099999999992</v>
       </c>
       <c r="C40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.71160356008116232</v>
       </c>
       <c r="D40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.1461596749473566</v>
       </c>
       <c r="E40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.64174387877723871</v>
       </c>
       <c r="F40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.039480335505665</v>
       </c>
       <c r="G40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.82798019576208692</v>
       </c>
       <c r="H40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.77861186700447282</v>
       </c>
       <c r="I40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.68213834916925731</v>
       </c>
       <c r="J40">
@@ -4146,13 +4142,13 @@
         <v>0</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="B41">
@@ -4160,31 +4156,31 @@
         <v>66.415300000000002</v>
       </c>
       <c r="C41">
-        <f t="shared" ref="C41:I42" si="10">C18/$B41</f>
+        <f t="shared" ref="C41:I42" si="11">C18/$B41</f>
         <v>3.686424664196352E-2</v>
       </c>
       <c r="D41">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0455422169289306</v>
       </c>
       <c r="E41">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.4466531055344175</v>
       </c>
       <c r="F41">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0333567717077241</v>
       </c>
       <c r="G41">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.5098117451852204E-2</v>
       </c>
       <c r="H41">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7.1954052755916181E-2</v>
       </c>
       <c r="I41">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.12788107559553294</v>
       </c>
       <c r="J41">
@@ -4212,13 +4208,13 @@
         <v>0</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="B42">
@@ -4226,31 +4222,31 @@
         <v>6.0363199999999999</v>
       </c>
       <c r="C42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.72394438995944543</v>
       </c>
       <c r="D42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>407.59104885095553</v>
       </c>
       <c r="E42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.67705986428817555</v>
       </c>
       <c r="F42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2896996845760331</v>
       </c>
       <c r="G42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.99913854798950352</v>
       </c>
       <c r="H42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.2612949611683941</v>
       </c>
       <c r="I42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.72056319081824682</v>
       </c>
       <c r="J42">
@@ -4278,45 +4274,45 @@
         <v>0</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="B43">
-        <f t="shared" ref="B43:B50" si="11">B21</f>
+        <f t="shared" ref="B43:B50" si="12">B21</f>
         <v>2.6436099999999998</v>
       </c>
       <c r="C43">
-        <f t="shared" ref="C43:I50" si="12">C21/$B43</f>
+        <f t="shared" ref="C43:I50" si="13">C21/$B43</f>
         <v>1.1227525996648522</v>
       </c>
       <c r="D43">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>990.32762018603353</v>
       </c>
       <c r="E43">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.64203872734631817</v>
       </c>
       <c r="F43">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.1630270728284431</v>
       </c>
       <c r="G43">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.52592099439781215</v>
       </c>
       <c r="H43">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>781.14018330994372</v>
       </c>
       <c r="I43">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>440.00817064544322</v>
       </c>
       <c r="J43">
@@ -4344,45 +4340,45 @@
         <v>0</v>
       </c>
       <c r="Q43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="B44">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.10762</v>
       </c>
       <c r="C44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.78653780177317123</v>
       </c>
       <c r="D44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5222.1068597533449</v>
       </c>
       <c r="E44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.72997959589028727</v>
       </c>
       <c r="F44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.1038081652552318</v>
       </c>
       <c r="G44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.78630848124808139</v>
       </c>
       <c r="H44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.3202993806540149</v>
       </c>
       <c r="I44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.81414203427168164</v>
       </c>
       <c r="J44">
@@ -4410,45 +4406,45 @@
         <v>0</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="B45">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7.0354400000000004</v>
       </c>
       <c r="C45">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.45332345951354852</v>
       </c>
       <c r="D45">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>112.92612828764085</v>
       </c>
       <c r="E45">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.3986260987230365</v>
       </c>
       <c r="F45">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.0305481959905847</v>
       </c>
       <c r="G45">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.43836917094026812</v>
       </c>
       <c r="H45">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>223.38617058776705</v>
       </c>
       <c r="I45">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>71.125473317944568</v>
       </c>
       <c r="J45">
@@ -4476,45 +4472,45 @@
         <v>0</v>
       </c>
       <c r="Q45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="B46">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.6732</v>
       </c>
       <c r="C46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.66207267511355483</v>
       </c>
       <c r="D46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>473.00083672005735</v>
       </c>
       <c r="E46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.60539086779823092</v>
       </c>
       <c r="F46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.91297513746115222</v>
       </c>
       <c r="G46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.62360148218981593</v>
       </c>
       <c r="H46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.76868276356681808</v>
       </c>
       <c r="I46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.6220953860865408</v>
       </c>
       <c r="J46">
@@ -4542,45 +4538,45 @@
         <v>0</v>
       </c>
       <c r="Q46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="B47">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>33.856299999999997</v>
       </c>
       <c r="C47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.0203270883114812</v>
       </c>
       <c r="D47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.5349314603190551</v>
       </c>
       <c r="E47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.66878837911998668</v>
       </c>
       <c r="F47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.1956179499827211</v>
       </c>
       <c r="G47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.9556448873621749</v>
       </c>
       <c r="H47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.91237081429453315</v>
       </c>
       <c r="I47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.67917049411778607</v>
       </c>
       <c r="J47">
@@ -4608,45 +4604,45 @@
         <v>0</v>
       </c>
       <c r="Q47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="B48">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7.9376499999999997</v>
       </c>
       <c r="C48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.89768508311653961</v>
       </c>
       <c r="D48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>11.365996233142052</v>
       </c>
       <c r="E48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.49476860279805734</v>
       </c>
       <c r="F48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.0389548543964524</v>
       </c>
       <c r="G48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.79712383388030461</v>
       </c>
       <c r="H48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.86411847335168468</v>
       </c>
       <c r="I48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.50579327634753357</v>
       </c>
       <c r="J48">
@@ -4674,45 +4670,45 @@
         <v>0</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
       <c r="B49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.46692</v>
       </c>
       <c r="C49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.7070937747116407</v>
       </c>
       <c r="D49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>164.74790717966897</v>
       </c>
       <c r="E49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.60787977531153714</v>
       </c>
       <c r="F49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.95003135821994389</v>
       </c>
       <c r="G49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.59870408747579962</v>
       </c>
       <c r="H49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.92709895563493572</v>
       </c>
       <c r="I49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.61485493414773817</v>
       </c>
       <c r="J49">
@@ -4740,45 +4736,45 @@
         <v>0</v>
       </c>
       <c r="Q49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="B50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.1663</v>
       </c>
       <c r="C50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.26105761191387228</v>
       </c>
       <c r="D50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.87934548459124762</v>
       </c>
       <c r="E50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.33517110453163884</v>
       </c>
       <c r="F50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.91901281685568992</v>
       </c>
       <c r="G50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.70207745197367777</v>
       </c>
       <c r="H50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.9787631685077169</v>
       </c>
       <c r="I50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>67.275016476004055</v>
       </c>
       <c r="J50">
@@ -4806,7 +4802,7 @@
         <v>0</v>
       </c>
       <c r="Q50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4819,65 +4815,65 @@
         <v>8.393461949999999</v>
       </c>
       <c r="C51">
-        <f t="shared" ref="C51:J51" si="13">AVERAGE(C31:C50)</f>
+        <f t="shared" ref="C51:J51" si="14">AVERAGE(C31:C50)</f>
         <v>0.66604467623809638</v>
       </c>
       <c r="D51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>391.31007556011195</v>
       </c>
       <c r="E51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.57793425048934832</v>
       </c>
       <c r="F51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.0265412990580025</v>
       </c>
       <c r="G51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.69861054100837083</v>
       </c>
       <c r="H51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>51.245589465792627</v>
       </c>
       <c r="I51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>29.447685191045753</v>
       </c>
       <c r="J51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.58341905726162235</v>
       </c>
-      <c r="L51" s="2" t="s">
+      <c r="L51" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M51" s="2">
+      <c r="M51" s="1">
         <f>AVERAGE(M31:M50)*100</f>
         <v>10</v>
       </c>
-      <c r="N51" s="2">
-        <f t="shared" ref="N51:R51" si="14">AVERAGE(N31:N50)*100</f>
-        <v>0</v>
-      </c>
-      <c r="O51" s="2">
-        <f t="shared" si="14"/>
+      <c r="N51" s="1">
+        <f t="shared" ref="N51:Q51" si="15">AVERAGE(N31:N50)*100</f>
+        <v>0</v>
+      </c>
+      <c r="O51" s="1">
+        <f t="shared" si="15"/>
         <v>60</v>
       </c>
-      <c r="P51" s="2">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="Q51" s="2">
-        <f t="shared" si="14"/>
-        <v>25</v>
-      </c>
-      <c r="R51" s="2">
+      <c r="P51" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Q51" s="1">
+        <f t="shared" si="15"/>
+        <v>30</v>
+      </c>
+      <c r="R51" s="1">
         <f>SUM(M51:Q51)</f>
-        <v>95</v>
-      </c>
-      <c r="S51" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="S51" s="1"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -4888,35 +4884,35 @@
         <v>8393.4599999999991</v>
       </c>
       <c r="C52">
-        <f t="shared" ref="C52:J52" si="15">ROUND(C51*1000,2)</f>
+        <f t="shared" ref="C52:J52" si="16">ROUND(C51*1000,2)</f>
         <v>666.04</v>
       </c>
       <c r="D52">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>391310.08000000002</v>
       </c>
       <c r="E52">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>577.92999999999995</v>
       </c>
       <c r="F52">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1026.54</v>
       </c>
       <c r="G52">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>698.61</v>
       </c>
       <c r="H52">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>51245.59</v>
       </c>
       <c r="I52">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>29447.69</v>
       </c>
       <c r="J52">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>583.41999999999996</v>
       </c>
     </row>

</xml_diff>